<commit_message>
RR Archive Data scraped and consolidated, assigned HP to the exisitng HP reference
</commit_message>
<xml_diff>
--- a/RR Picture Archives List.xlsx
+++ b/RR Picture Archives List.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dshi\Documents\GitHub\Web-Scraping\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ds57534\Documents\GitHub\Web-Scraping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0977D953-B915-43CC-B210-9BA48C9EBB2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BA7C998-FFE7-4269-A7F6-424BAB228AFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{E4EE507A-2BA0-4F7A-AA93-07851E16F37B}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{E4EE507A-2BA0-4F7A-AA93-07851E16F37B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,8 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -38,9 +36,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="253">
   <si>
-    <t>Reporting Marks  </t>
-  </si>
-  <si>
     <t>Railroad name</t>
   </si>
   <si>
@@ -795,13 +790,16 @@
   </si>
   <si>
     <t>Weyerhauser</t>
+  </si>
+  <si>
+    <t>Reporting Marks</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1169,48 +1167,48 @@
   <dimension ref="A1:D126"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="2" max="2" width="33.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>252</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>223</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>224</v>
       </c>
       <c r="C2">
         <v>298</v>
       </c>
       <c r="D2">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B3" t="s">
         <v>192</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
       </c>
       <c r="C3">
         <v>219</v>
@@ -1219,12 +1217,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>231</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>232</v>
       </c>
       <c r="C4">
         <v>158</v>
@@ -1233,12 +1231,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>225</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>226</v>
       </c>
       <c r="C5">
         <v>106</v>
@@ -1247,12 +1245,12 @@
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>49</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>50</v>
       </c>
       <c r="C6">
         <v>94</v>
@@ -1261,12 +1259,12 @@
         <v>3353</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>203</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>204</v>
       </c>
       <c r="C7">
         <v>80</v>
@@ -1275,12 +1273,12 @@
         <v>90</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>189</v>
       </c>
       <c r="B8" t="s">
-        <v>17</v>
+        <v>190</v>
       </c>
       <c r="C8">
         <v>76</v>
@@ -1289,12 +1287,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>209</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
+        <v>210</v>
       </c>
       <c r="C9">
         <v>70</v>
@@ -1303,12 +1301,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>221</v>
       </c>
       <c r="B10" t="s">
-        <v>21</v>
+        <v>222</v>
       </c>
       <c r="C10">
         <v>69</v>
@@ -1317,12 +1315,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>22</v>
+        <v>107</v>
       </c>
       <c r="B11" t="s">
-        <v>23</v>
+        <v>108</v>
       </c>
       <c r="C11">
         <v>60</v>
@@ -1331,12 +1329,12 @@
         <v>430</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>24</v>
+        <v>229</v>
       </c>
       <c r="B12" t="s">
-        <v>25</v>
+        <v>230</v>
       </c>
       <c r="C12">
         <v>51</v>
@@ -1345,12 +1343,12 @@
         <v>64</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>26</v>
+        <v>157</v>
       </c>
       <c r="B13" t="s">
-        <v>27</v>
+        <v>158</v>
       </c>
       <c r="C13">
         <v>39</v>
@@ -1359,12 +1357,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>28</v>
+        <v>227</v>
       </c>
       <c r="B14" t="s">
-        <v>29</v>
+        <v>228</v>
       </c>
       <c r="C14">
         <v>37</v>
@@ -1373,12 +1371,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>30</v>
+        <v>55</v>
       </c>
       <c r="B15" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="C15">
         <v>35</v>
@@ -1387,12 +1385,12 @@
         <v>48</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>32</v>
+        <v>141</v>
       </c>
       <c r="B16" t="s">
-        <v>33</v>
+        <v>142</v>
       </c>
       <c r="C16">
         <v>34</v>
@@ -1401,12 +1399,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>34</v>
+        <v>250</v>
       </c>
       <c r="B17" t="s">
-        <v>35</v>
+        <v>251</v>
       </c>
       <c r="C17">
         <v>29</v>
@@ -1415,12 +1413,12 @@
         <v>53</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>36</v>
+        <v>143</v>
       </c>
       <c r="B18" t="s">
-        <v>37</v>
+        <v>144</v>
       </c>
       <c r="C18">
         <v>28</v>
@@ -1429,12 +1427,12 @@
         <v>207</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>38</v>
+        <v>238</v>
       </c>
       <c r="B19" t="s">
-        <v>39</v>
+        <v>239</v>
       </c>
       <c r="C19">
         <v>27</v>
@@ -1443,12 +1441,12 @@
         <v>509</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>40</v>
+        <v>119</v>
       </c>
       <c r="B20" t="s">
-        <v>41</v>
+        <v>120</v>
       </c>
       <c r="C20">
         <v>26</v>
@@ -1457,12 +1455,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>42</v>
+        <v>155</v>
       </c>
       <c r="B21" t="s">
-        <v>43</v>
+        <v>156</v>
       </c>
       <c r="C21">
         <v>25</v>
@@ -1471,12 +1469,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4">
       <c r="A22" t="s">
-        <v>44</v>
+        <v>248</v>
       </c>
       <c r="B22" t="s">
-        <v>45</v>
+        <v>249</v>
       </c>
       <c r="C22">
         <v>24</v>
@@ -1485,12 +1483,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>46</v>
+        <v>145</v>
       </c>
       <c r="B23" t="s">
-        <v>47</v>
+        <v>146</v>
       </c>
       <c r="C23">
         <v>23</v>
@@ -1499,12 +1497,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>48</v>
+        <v>77</v>
       </c>
       <c r="B24" t="s">
-        <v>49</v>
+        <v>78</v>
       </c>
       <c r="C24">
         <v>20</v>
@@ -1513,12 +1511,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>50</v>
+        <v>3</v>
       </c>
       <c r="B25" t="s">
-        <v>51</v>
+        <v>4</v>
       </c>
       <c r="C25">
         <v>18</v>
@@ -1527,12 +1525,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4">
       <c r="A26" t="s">
-        <v>52</v>
+        <v>17</v>
       </c>
       <c r="B26" t="s">
-        <v>53</v>
+        <v>18</v>
       </c>
       <c r="C26">
         <v>16</v>
@@ -1541,12 +1539,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4">
       <c r="A27" t="s">
-        <v>54</v>
+        <v>244</v>
       </c>
       <c r="B27" t="s">
-        <v>55</v>
+        <v>245</v>
       </c>
       <c r="C27">
         <v>16</v>
@@ -1555,12 +1553,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4">
       <c r="A28" t="s">
-        <v>56</v>
+        <v>89</v>
       </c>
       <c r="B28" t="s">
-        <v>57</v>
+        <v>90</v>
       </c>
       <c r="C28">
         <v>15</v>
@@ -1569,12 +1567,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:4">
       <c r="A29" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="B29" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="C29">
         <v>14</v>
@@ -1583,12 +1581,12 @@
         <v>202</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4">
       <c r="A30" t="s">
-        <v>60</v>
+        <v>15</v>
       </c>
       <c r="B30" t="s">
-        <v>61</v>
+        <v>16</v>
       </c>
       <c r="C30">
         <v>13</v>
@@ -1597,12 +1595,12 @@
         <v>79</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:4">
       <c r="A31" t="s">
-        <v>62</v>
+        <v>41</v>
       </c>
       <c r="B31" t="s">
-        <v>63</v>
+        <v>42</v>
       </c>
       <c r="C31">
         <v>13</v>
@@ -1611,12 +1609,12 @@
         <v>232</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:4">
       <c r="A32" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B32" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C32">
         <v>12</v>
@@ -1625,12 +1623,12 @@
         <v>236</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:4">
       <c r="A33" t="s">
-        <v>66</v>
+        <v>173</v>
       </c>
       <c r="B33" t="s">
-        <v>67</v>
+        <v>174</v>
       </c>
       <c r="C33">
         <v>12</v>
@@ -1639,12 +1637,12 @@
         <v>92</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:4">
       <c r="A34" t="s">
-        <v>68</v>
+        <v>183</v>
       </c>
       <c r="B34" t="s">
-        <v>69</v>
+        <v>184</v>
       </c>
       <c r="C34">
         <v>12</v>
@@ -1653,12 +1651,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:4">
       <c r="A35" t="s">
-        <v>70</v>
+        <v>147</v>
       </c>
       <c r="B35" t="s">
-        <v>71</v>
+        <v>148</v>
       </c>
       <c r="C35">
         <v>11</v>
@@ -1667,12 +1665,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:4">
       <c r="A36" t="s">
-        <v>72</v>
+        <v>242</v>
       </c>
       <c r="B36" t="s">
-        <v>73</v>
+        <v>243</v>
       </c>
       <c r="C36">
         <v>11</v>
@@ -1681,12 +1679,12 @@
         <v>199</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:4">
       <c r="A37" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="B37" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="C37">
         <v>10</v>
@@ -1695,12 +1693,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:4">
       <c r="A38" t="s">
-        <v>76</v>
+        <v>115</v>
       </c>
       <c r="B38" t="s">
-        <v>77</v>
+        <v>116</v>
       </c>
       <c r="C38">
         <v>10</v>
@@ -1709,12 +1707,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:4">
       <c r="A39" t="s">
-        <v>78</v>
+        <v>201</v>
       </c>
       <c r="B39" t="s">
-        <v>79</v>
+        <v>202</v>
       </c>
       <c r="C39">
         <v>10</v>
@@ -1723,12 +1721,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:4">
       <c r="A40" t="s">
+        <v>79</v>
+      </c>
+      <c r="B40" t="s">
         <v>80</v>
-      </c>
-      <c r="B40" t="s">
-        <v>81</v>
       </c>
       <c r="C40">
         <v>9</v>
@@ -1737,12 +1735,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:4">
       <c r="A41" t="s">
-        <v>82</v>
+        <v>129</v>
       </c>
       <c r="B41" t="s">
-        <v>83</v>
+        <v>130</v>
       </c>
       <c r="C41">
         <v>9</v>
@@ -1751,12 +1749,12 @@
         <v>430</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:4">
       <c r="A42" t="s">
-        <v>84</v>
+        <v>137</v>
       </c>
       <c r="B42" t="s">
-        <v>85</v>
+        <v>138</v>
       </c>
       <c r="C42">
         <v>9</v>
@@ -1765,12 +1763,12 @@
         <v>86</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:4">
       <c r="A43" t="s">
-        <v>86</v>
+        <v>246</v>
       </c>
       <c r="B43" t="s">
-        <v>87</v>
+        <v>247</v>
       </c>
       <c r="C43">
         <v>9</v>
@@ -1779,12 +1777,12 @@
         <v>692</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:4">
       <c r="A44" t="s">
-        <v>88</v>
+        <v>53</v>
       </c>
       <c r="B44" t="s">
-        <v>89</v>
+        <v>54</v>
       </c>
       <c r="C44">
         <v>8</v>
@@ -1793,12 +1791,12 @@
         <v>2159</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:4">
       <c r="A45" t="s">
-        <v>90</v>
+        <v>65</v>
       </c>
       <c r="B45" t="s">
-        <v>91</v>
+        <v>66</v>
       </c>
       <c r="C45">
         <v>8</v>
@@ -1807,12 +1805,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:4">
       <c r="A46" t="s">
-        <v>92</v>
+        <v>125</v>
       </c>
       <c r="B46" t="s">
-        <v>93</v>
+        <v>126</v>
       </c>
       <c r="C46">
         <v>8</v>
@@ -1821,12 +1819,12 @@
         <v>414</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:4">
       <c r="A47" t="s">
-        <v>94</v>
+        <v>165</v>
       </c>
       <c r="B47" t="s">
-        <v>95</v>
+        <v>166</v>
       </c>
       <c r="C47">
         <v>8</v>
@@ -1835,26 +1833,26 @@
         <v>3</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:4">
       <c r="A48" t="s">
-        <v>96</v>
+        <v>235</v>
       </c>
       <c r="B48" t="s">
-        <v>97</v>
+        <v>234</v>
       </c>
       <c r="C48">
         <v>8</v>
       </c>
       <c r="D48">
-        <v>28843</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
+        <v>28845</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
       <c r="A49" t="s">
-        <v>98</v>
+        <v>7</v>
       </c>
       <c r="B49" t="s">
-        <v>99</v>
+        <v>8</v>
       </c>
       <c r="C49">
         <v>7</v>
@@ -1863,12 +1861,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:4">
       <c r="A50" t="s">
-        <v>100</v>
+        <v>151</v>
       </c>
       <c r="B50" t="s">
-        <v>101</v>
+        <v>152</v>
       </c>
       <c r="C50">
         <v>7</v>
@@ -1877,12 +1875,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:4">
       <c r="A51" t="s">
-        <v>102</v>
+        <v>187</v>
       </c>
       <c r="B51" t="s">
-        <v>103</v>
+        <v>188</v>
       </c>
       <c r="C51">
         <v>7</v>
@@ -1891,12 +1889,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:4">
       <c r="A52" t="s">
-        <v>104</v>
+        <v>205</v>
       </c>
       <c r="B52" t="s">
-        <v>105</v>
+        <v>206</v>
       </c>
       <c r="C52">
         <v>7</v>
@@ -1905,12 +1903,12 @@
         <v>48</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:4">
       <c r="A53" t="s">
-        <v>106</v>
+        <v>215</v>
       </c>
       <c r="B53" t="s">
-        <v>107</v>
+        <v>216</v>
       </c>
       <c r="C53">
         <v>7</v>
@@ -1919,12 +1917,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:4">
       <c r="A54" t="s">
-        <v>108</v>
+        <v>9</v>
       </c>
       <c r="B54" t="s">
-        <v>109</v>
+        <v>10</v>
       </c>
       <c r="C54">
         <v>6</v>
@@ -1933,12 +1931,12 @@
         <v>2262</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:4">
       <c r="A55" t="s">
-        <v>110</v>
+        <v>57</v>
       </c>
       <c r="B55" t="s">
-        <v>111</v>
+        <v>58</v>
       </c>
       <c r="C55">
         <v>6</v>
@@ -1947,12 +1945,12 @@
         <v>165</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:4">
       <c r="A56" t="s">
-        <v>112</v>
+        <v>197</v>
       </c>
       <c r="B56" t="s">
-        <v>113</v>
+        <v>198</v>
       </c>
       <c r="C56">
         <v>6</v>
@@ -1961,26 +1959,26 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:4">
       <c r="A57" t="s">
-        <v>114</v>
+        <v>233</v>
       </c>
       <c r="B57" t="s">
-        <v>115</v>
+        <v>234</v>
       </c>
       <c r="C57">
         <v>6</v>
       </c>
       <c r="D57">
-        <v>2858</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
+        <v>2859</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4">
       <c r="A58" t="s">
-        <v>116</v>
+        <v>236</v>
       </c>
       <c r="B58" t="s">
-        <v>117</v>
+        <v>237</v>
       </c>
       <c r="C58">
         <v>6</v>
@@ -1989,12 +1987,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:4">
       <c r="A59" t="s">
-        <v>118</v>
+        <v>5</v>
       </c>
       <c r="B59" t="s">
-        <v>119</v>
+        <v>6</v>
       </c>
       <c r="C59">
         <v>5</v>
@@ -2003,12 +2001,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:4">
       <c r="A60" t="s">
-        <v>120</v>
+        <v>85</v>
       </c>
       <c r="B60" t="s">
-        <v>121</v>
+        <v>86</v>
       </c>
       <c r="C60">
         <v>5</v>
@@ -2017,12 +2015,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:4">
       <c r="A61" t="s">
-        <v>122</v>
+        <v>211</v>
       </c>
       <c r="B61" t="s">
-        <v>123</v>
+        <v>212</v>
       </c>
       <c r="C61">
         <v>5</v>
@@ -2031,12 +2029,12 @@
         <v>236</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:4">
       <c r="A62" t="s">
-        <v>124</v>
+        <v>217</v>
       </c>
       <c r="B62" t="s">
-        <v>125</v>
+        <v>218</v>
       </c>
       <c r="C62">
         <v>5</v>
@@ -2045,12 +2043,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:4">
       <c r="A63" t="s">
-        <v>126</v>
+        <v>23</v>
       </c>
       <c r="B63" t="s">
-        <v>127</v>
+        <v>24</v>
       </c>
       <c r="C63">
         <v>4</v>
@@ -2059,12 +2057,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:4">
       <c r="A64" t="s">
-        <v>128</v>
+        <v>33</v>
       </c>
       <c r="B64" t="s">
-        <v>129</v>
+        <v>34</v>
       </c>
       <c r="C64">
         <v>4</v>
@@ -2073,12 +2071,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:4">
       <c r="A65" t="s">
-        <v>130</v>
+        <v>69</v>
       </c>
       <c r="B65" t="s">
-        <v>131</v>
+        <v>70</v>
       </c>
       <c r="C65">
         <v>4</v>
@@ -2087,12 +2085,12 @@
         <v>721</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:4">
       <c r="A66" t="s">
-        <v>132</v>
+        <v>71</v>
       </c>
       <c r="B66" t="s">
-        <v>133</v>
+        <v>72</v>
       </c>
       <c r="C66">
         <v>4</v>
@@ -2101,12 +2099,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:4">
       <c r="A67" t="s">
-        <v>134</v>
+        <v>21</v>
       </c>
       <c r="B67" t="s">
-        <v>135</v>
+        <v>22</v>
       </c>
       <c r="C67">
         <v>3</v>
@@ -2115,12 +2113,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:4">
       <c r="A68" t="s">
-        <v>136</v>
+        <v>25</v>
       </c>
       <c r="B68" t="s">
-        <v>137</v>
+        <v>26</v>
       </c>
       <c r="C68">
         <v>3</v>
@@ -2129,12 +2127,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:4">
       <c r="A69" t="s">
-        <v>138</v>
+        <v>35</v>
       </c>
       <c r="B69" t="s">
-        <v>139</v>
+        <v>36</v>
       </c>
       <c r="C69">
         <v>3</v>
@@ -2143,12 +2141,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:4">
       <c r="A70" t="s">
-        <v>140</v>
+        <v>39</v>
       </c>
       <c r="B70" t="s">
-        <v>141</v>
+        <v>40</v>
       </c>
       <c r="C70">
         <v>3</v>
@@ -2157,12 +2155,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:4">
       <c r="A71" t="s">
-        <v>142</v>
+        <v>45</v>
       </c>
       <c r="B71" t="s">
-        <v>143</v>
+        <v>46</v>
       </c>
       <c r="C71">
         <v>3</v>
@@ -2171,12 +2169,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:4">
       <c r="A72" t="s">
-        <v>144</v>
+        <v>67</v>
       </c>
       <c r="B72" t="s">
-        <v>145</v>
+        <v>68</v>
       </c>
       <c r="C72">
         <v>3</v>
@@ -2185,12 +2183,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:4">
       <c r="A73" t="s">
-        <v>146</v>
+        <v>73</v>
       </c>
       <c r="B73" t="s">
-        <v>147</v>
+        <v>74</v>
       </c>
       <c r="C73">
         <v>3</v>
@@ -2199,12 +2197,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:4">
       <c r="A74" t="s">
-        <v>148</v>
+        <v>95</v>
       </c>
       <c r="B74" t="s">
-        <v>149</v>
+        <v>96</v>
       </c>
       <c r="C74">
         <v>3</v>
@@ -2213,12 +2211,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:4">
       <c r="A75" t="s">
-        <v>150</v>
+        <v>99</v>
       </c>
       <c r="B75" t="s">
-        <v>151</v>
+        <v>100</v>
       </c>
       <c r="C75">
         <v>3</v>
@@ -2227,12 +2225,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:4">
       <c r="A76" t="s">
-        <v>152</v>
+        <v>109</v>
       </c>
       <c r="B76" t="s">
-        <v>153</v>
+        <v>110</v>
       </c>
       <c r="C76">
         <v>3</v>
@@ -2241,12 +2239,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:4">
       <c r="A77" t="s">
-        <v>154</v>
+        <v>117</v>
       </c>
       <c r="B77" t="s">
-        <v>155</v>
+        <v>118</v>
       </c>
       <c r="C77">
         <v>3</v>
@@ -2255,12 +2253,12 @@
         <v>225</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:4">
       <c r="A78" t="s">
-        <v>156</v>
+        <v>127</v>
       </c>
       <c r="B78" t="s">
-        <v>157</v>
+        <v>128</v>
       </c>
       <c r="C78">
         <v>3</v>
@@ -2269,12 +2267,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:4">
       <c r="A79" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B79" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C79">
         <v>3</v>
@@ -2283,12 +2281,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:4">
       <c r="A80" t="s">
-        <v>160</v>
+        <v>179</v>
       </c>
       <c r="B80" t="s">
-        <v>161</v>
+        <v>180</v>
       </c>
       <c r="C80">
         <v>3</v>
@@ -2297,12 +2295,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:4">
       <c r="A81" t="s">
-        <v>162</v>
+        <v>181</v>
       </c>
       <c r="B81" t="s">
-        <v>163</v>
+        <v>182</v>
       </c>
       <c r="C81">
         <v>3</v>
@@ -2311,12 +2309,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:4">
       <c r="A82" t="s">
-        <v>164</v>
+        <v>193</v>
       </c>
       <c r="B82" t="s">
-        <v>165</v>
+        <v>194</v>
       </c>
       <c r="C82">
         <v>3</v>
@@ -2325,12 +2323,12 @@
         <v>27</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:4">
       <c r="A83" t="s">
-        <v>166</v>
+        <v>195</v>
       </c>
       <c r="B83" t="s">
-        <v>167</v>
+        <v>196</v>
       </c>
       <c r="C83">
         <v>3</v>
@@ -2339,12 +2337,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:4">
       <c r="A84" t="s">
-        <v>168</v>
+        <v>213</v>
       </c>
       <c r="B84" t="s">
-        <v>169</v>
+        <v>214</v>
       </c>
       <c r="C84">
         <v>3</v>
@@ -2353,12 +2351,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:4">
       <c r="A85" t="s">
-        <v>170</v>
+        <v>11</v>
       </c>
       <c r="B85" t="s">
-        <v>171</v>
+        <v>12</v>
       </c>
       <c r="C85">
         <v>2</v>
@@ -2367,12 +2365,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:4">
       <c r="A86" t="s">
-        <v>172</v>
+        <v>19</v>
       </c>
       <c r="B86" t="s">
-        <v>173</v>
+        <v>20</v>
       </c>
       <c r="C86">
         <v>2</v>
@@ -2381,12 +2379,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:4">
       <c r="A87" t="s">
-        <v>174</v>
+        <v>51</v>
       </c>
       <c r="B87" t="s">
-        <v>175</v>
+        <v>52</v>
       </c>
       <c r="C87">
         <v>2</v>
@@ -2395,12 +2393,12 @@
         <v>565</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:4">
       <c r="A88" t="s">
-        <v>176</v>
+        <v>63</v>
       </c>
       <c r="B88" t="s">
-        <v>177</v>
+        <v>64</v>
       </c>
       <c r="C88">
         <v>2</v>
@@ -2409,12 +2407,12 @@
         <v>1482</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:4">
       <c r="A89" t="s">
-        <v>178</v>
+        <v>97</v>
       </c>
       <c r="B89" t="s">
-        <v>179</v>
+        <v>98</v>
       </c>
       <c r="C89">
         <v>2</v>
@@ -2423,12 +2421,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:4">
       <c r="A90" t="s">
-        <v>180</v>
+        <v>121</v>
       </c>
       <c r="B90" t="s">
-        <v>181</v>
+        <v>122</v>
       </c>
       <c r="C90">
         <v>2</v>
@@ -2437,12 +2435,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:4">
       <c r="A91" t="s">
-        <v>182</v>
+        <v>133</v>
       </c>
       <c r="B91" t="s">
-        <v>183</v>
+        <v>134</v>
       </c>
       <c r="C91">
         <v>2</v>
@@ -2451,12 +2449,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:4">
       <c r="A92" t="s">
-        <v>184</v>
+        <v>139</v>
       </c>
       <c r="B92" t="s">
-        <v>185</v>
+        <v>140</v>
       </c>
       <c r="C92">
         <v>2</v>
@@ -2465,12 +2463,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:4">
       <c r="A93" t="s">
-        <v>186</v>
+        <v>153</v>
       </c>
       <c r="B93" t="s">
-        <v>187</v>
+        <v>154</v>
       </c>
       <c r="C93">
         <v>2</v>
@@ -2479,12 +2477,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:4">
       <c r="A94" t="s">
-        <v>188</v>
+        <v>163</v>
       </c>
       <c r="B94" t="s">
-        <v>189</v>
+        <v>164</v>
       </c>
       <c r="C94">
         <v>2</v>
@@ -2493,12 +2491,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:4">
       <c r="A95" t="s">
-        <v>190</v>
+        <v>167</v>
       </c>
       <c r="B95" t="s">
-        <v>191</v>
+        <v>168</v>
       </c>
       <c r="C95">
         <v>2</v>
@@ -2507,12 +2505,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:4">
       <c r="A96" t="s">
-        <v>192</v>
+        <v>169</v>
       </c>
       <c r="B96" t="s">
-        <v>193</v>
+        <v>170</v>
       </c>
       <c r="C96">
         <v>2</v>
@@ -2521,12 +2519,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:4">
       <c r="A97" t="s">
-        <v>194</v>
+        <v>175</v>
       </c>
       <c r="B97" t="s">
-        <v>195</v>
+        <v>176</v>
       </c>
       <c r="C97">
         <v>2</v>
@@ -2535,12 +2533,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:4">
       <c r="A98" t="s">
-        <v>196</v>
+        <v>177</v>
       </c>
       <c r="B98" t="s">
-        <v>197</v>
+        <v>178</v>
       </c>
       <c r="C98">
         <v>2</v>
@@ -2549,12 +2547,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:4">
       <c r="A99" t="s">
-        <v>198</v>
+        <v>219</v>
       </c>
       <c r="B99" t="s">
-        <v>199</v>
+        <v>220</v>
       </c>
       <c r="C99">
         <v>2</v>
@@ -2563,12 +2561,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:4">
       <c r="A100" t="s">
-        <v>200</v>
+        <v>13</v>
       </c>
       <c r="B100" t="s">
-        <v>201</v>
+        <v>14</v>
       </c>
       <c r="C100">
         <v>1</v>
@@ -2577,12 +2575,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:4">
       <c r="A101" t="s">
-        <v>202</v>
+        <v>27</v>
       </c>
       <c r="B101" t="s">
-        <v>203</v>
+        <v>28</v>
       </c>
       <c r="C101">
         <v>1</v>
@@ -2591,12 +2589,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:4">
       <c r="A102" t="s">
-        <v>204</v>
+        <v>31</v>
       </c>
       <c r="B102" t="s">
-        <v>205</v>
+        <v>32</v>
       </c>
       <c r="C102">
         <v>1</v>
@@ -2605,12 +2603,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:4">
       <c r="A103" t="s">
-        <v>206</v>
+        <v>37</v>
       </c>
       <c r="B103" t="s">
-        <v>207</v>
+        <v>38</v>
       </c>
       <c r="C103">
         <v>1</v>
@@ -2619,12 +2617,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:4">
       <c r="A104" t="s">
-        <v>208</v>
+        <v>47</v>
       </c>
       <c r="B104" t="s">
-        <v>209</v>
+        <v>48</v>
       </c>
       <c r="C104">
         <v>1</v>
@@ -2633,12 +2631,12 @@
         <v>551</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:4">
       <c r="A105" t="s">
-        <v>210</v>
+        <v>59</v>
       </c>
       <c r="B105" t="s">
-        <v>211</v>
+        <v>60</v>
       </c>
       <c r="C105">
         <v>1</v>
@@ -2647,12 +2645,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:4">
       <c r="A106" t="s">
-        <v>212</v>
+        <v>75</v>
       </c>
       <c r="B106" t="s">
-        <v>213</v>
+        <v>76</v>
       </c>
       <c r="C106">
         <v>1</v>
@@ -2661,12 +2659,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:4">
       <c r="A107" t="s">
-        <v>214</v>
+        <v>87</v>
       </c>
       <c r="B107" t="s">
-        <v>215</v>
+        <v>88</v>
       </c>
       <c r="C107">
         <v>1</v>
@@ -2675,12 +2673,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:4">
       <c r="A108" t="s">
-        <v>216</v>
+        <v>91</v>
       </c>
       <c r="B108" t="s">
-        <v>217</v>
+        <v>92</v>
       </c>
       <c r="C108">
         <v>1</v>
@@ -2689,12 +2687,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:4">
       <c r="A109" t="s">
-        <v>218</v>
+        <v>93</v>
       </c>
       <c r="B109" t="s">
-        <v>219</v>
+        <v>94</v>
       </c>
       <c r="C109">
         <v>1</v>
@@ -2703,12 +2701,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:4">
       <c r="A110" t="s">
-        <v>220</v>
+        <v>101</v>
       </c>
       <c r="B110" t="s">
-        <v>221</v>
+        <v>102</v>
       </c>
       <c r="C110">
         <v>1</v>
@@ -2717,12 +2715,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:4">
       <c r="A111" t="s">
-        <v>222</v>
+        <v>103</v>
       </c>
       <c r="B111" t="s">
-        <v>223</v>
+        <v>104</v>
       </c>
       <c r="C111">
         <v>1</v>
@@ -2731,12 +2729,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:4">
       <c r="A112" t="s">
-        <v>224</v>
+        <v>105</v>
       </c>
       <c r="B112" t="s">
-        <v>225</v>
+        <v>106</v>
       </c>
       <c r="C112">
         <v>1</v>
@@ -2745,12 +2743,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:4">
       <c r="A113" t="s">
-        <v>226</v>
+        <v>111</v>
       </c>
       <c r="B113" t="s">
-        <v>227</v>
+        <v>112</v>
       </c>
       <c r="C113">
         <v>1</v>
@@ -2759,12 +2757,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:4">
       <c r="A114" t="s">
-        <v>228</v>
+        <v>113</v>
       </c>
       <c r="B114" t="s">
-        <v>229</v>
+        <v>114</v>
       </c>
       <c r="C114">
         <v>1</v>
@@ -2773,12 +2771,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:4">
       <c r="A115" t="s">
-        <v>230</v>
+        <v>131</v>
       </c>
       <c r="B115" t="s">
-        <v>231</v>
+        <v>132</v>
       </c>
       <c r="C115">
         <v>1</v>
@@ -2787,12 +2785,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:4">
       <c r="A116" t="s">
-        <v>232</v>
+        <v>135</v>
       </c>
       <c r="B116" t="s">
-        <v>233</v>
+        <v>136</v>
       </c>
       <c r="C116">
         <v>1</v>
@@ -2801,12 +2799,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:4">
       <c r="A117" t="s">
-        <v>234</v>
+        <v>161</v>
       </c>
       <c r="B117" t="s">
-        <v>235</v>
+        <v>162</v>
       </c>
       <c r="C117">
         <v>1</v>
@@ -2815,12 +2813,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:4">
       <c r="A118" t="s">
-        <v>236</v>
+        <v>171</v>
       </c>
       <c r="B118" t="s">
-        <v>235</v>
+        <v>172</v>
       </c>
       <c r="C118">
         <v>1</v>
@@ -2829,12 +2827,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:4">
       <c r="A119" t="s">
-        <v>237</v>
+        <v>185</v>
       </c>
       <c r="B119" t="s">
-        <v>238</v>
+        <v>186</v>
       </c>
       <c r="C119">
         <v>1</v>
@@ -2843,27 +2841,27 @@
         <v>2</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:4">
       <c r="A120" t="s">
-        <v>239</v>
+        <v>199</v>
       </c>
       <c r="B120" t="s">
+        <v>200</v>
+      </c>
+      <c r="C120">
+        <v>1</v>
+      </c>
+      <c r="D120">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4">
+      <c r="A121" t="s">
         <v>240</v>
       </c>
-      <c r="C120">
-        <v>1</v>
-      </c>
-      <c r="D120">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A121" t="s">
+      <c r="B121" t="s">
         <v>241</v>
       </c>
-      <c r="B121" t="s">
-        <v>242</v>
-      </c>
       <c r="C121">
         <v>1</v>
       </c>
@@ -2871,12 +2869,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:4">
       <c r="A122" t="s">
-        <v>243</v>
+        <v>29</v>
       </c>
       <c r="B122" t="s">
-        <v>244</v>
+        <v>30</v>
       </c>
       <c r="C122">
         <v>0</v>
@@ -2885,12 +2883,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:4">
       <c r="A123" t="s">
-        <v>245</v>
+        <v>83</v>
       </c>
       <c r="B123" t="s">
-        <v>246</v>
+        <v>84</v>
       </c>
       <c r="C123">
         <v>0</v>
@@ -2899,12 +2897,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:4">
       <c r="A124" t="s">
-        <v>247</v>
+        <v>123</v>
       </c>
       <c r="B124" t="s">
-        <v>248</v>
+        <v>124</v>
       </c>
       <c r="C124">
         <v>0</v>
@@ -2913,12 +2911,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:4">
       <c r="A125" t="s">
-        <v>249</v>
+        <v>149</v>
       </c>
       <c r="B125" t="s">
-        <v>250</v>
+        <v>150</v>
       </c>
       <c r="C125">
         <v>0</v>
@@ -2927,12 +2925,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:4">
       <c r="A126" t="s">
-        <v>251</v>
+        <v>207</v>
       </c>
       <c r="B126" t="s">
-        <v>252</v>
+        <v>208</v>
       </c>
       <c r="C126">
         <v>0</v>
@@ -2942,10 +2940,11 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C2:D126">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D126">
     <sortCondition descending="1" ref="C1:C126"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Added company name for RR data, added acquisition date and reporting marks for CGdata
</commit_message>
<xml_diff>
--- a/RR Picture Archives List.xlsx
+++ b/RR Picture Archives List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ds57534\Documents\GitHub\Web-Scraping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BA7C998-FFE7-4269-A7F6-424BAB228AFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A74484D6-9D74-485F-9F6C-F6776F9054B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{E4EE507A-2BA0-4F7A-AA93-07851E16F37B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{E4EE507A-2BA0-4F7A-AA93-07851E16F37B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -57,9 +57,6 @@
     <t>Alabama Byproducts Corporation</t>
   </si>
   <si>
-    <t>Acme</t>
-  </si>
-  <si>
     <t>Acme Steel</t>
   </si>
   <si>
@@ -793,6 +790,9 @@
   </si>
   <si>
     <t>Reporting Marks</t>
+  </si>
+  <si>
+    <t>ACME</t>
   </si>
 </sst>
 </file>
@@ -1167,7 +1167,7 @@
   <dimension ref="A1:D126"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1177,7 +1177,7 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -1191,209 +1191,209 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>223</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>224</v>
+        <v>4</v>
       </c>
       <c r="C2">
-        <v>298</v>
+        <v>18</v>
       </c>
       <c r="D2">
-        <v>195</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>191</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>192</v>
+        <v>6</v>
       </c>
       <c r="C3">
-        <v>219</v>
+        <v>5</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>231</v>
+        <v>252</v>
       </c>
       <c r="B4" t="s">
-        <v>232</v>
+        <v>7</v>
       </c>
       <c r="C4">
-        <v>158</v>
+        <v>7</v>
       </c>
       <c r="D4">
-        <v>15</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>225</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>226</v>
+        <v>9</v>
       </c>
       <c r="C5">
-        <v>106</v>
+        <v>6</v>
       </c>
       <c r="D5">
-        <v>48</v>
+        <v>2262</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>49</v>
+        <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>50</v>
+        <v>11</v>
       </c>
       <c r="C6">
-        <v>94</v>
+        <v>2</v>
       </c>
       <c r="D6">
-        <v>3353</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>203</v>
+        <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>204</v>
+        <v>13</v>
       </c>
       <c r="C7">
-        <v>80</v>
+        <v>1</v>
       </c>
       <c r="D7">
-        <v>90</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>189</v>
+        <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>190</v>
+        <v>15</v>
       </c>
       <c r="C8">
-        <v>76</v>
+        <v>13</v>
       </c>
       <c r="D8">
-        <v>0</v>
+        <v>79</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>209</v>
+        <v>16</v>
       </c>
       <c r="B9" t="s">
-        <v>210</v>
+        <v>17</v>
       </c>
       <c r="C9">
-        <v>70</v>
+        <v>16</v>
       </c>
       <c r="D9">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>221</v>
+        <v>18</v>
       </c>
       <c r="B10" t="s">
-        <v>222</v>
+        <v>19</v>
       </c>
       <c r="C10">
-        <v>69</v>
+        <v>2</v>
       </c>
       <c r="D10">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>107</v>
+        <v>20</v>
       </c>
       <c r="B11" t="s">
-        <v>108</v>
+        <v>21</v>
       </c>
       <c r="C11">
-        <v>60</v>
+        <v>3</v>
       </c>
       <c r="D11">
-        <v>430</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>229</v>
+        <v>22</v>
       </c>
       <c r="B12" t="s">
-        <v>230</v>
+        <v>23</v>
       </c>
       <c r="C12">
-        <v>51</v>
+        <v>4</v>
       </c>
       <c r="D12">
-        <v>64</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>157</v>
+        <v>24</v>
       </c>
       <c r="B13" t="s">
-        <v>158</v>
+        <v>25</v>
       </c>
       <c r="C13">
-        <v>39</v>
+        <v>3</v>
       </c>
       <c r="D13">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>227</v>
+        <v>26</v>
       </c>
       <c r="B14" t="s">
-        <v>228</v>
+        <v>27</v>
       </c>
       <c r="C14">
-        <v>37</v>
+        <v>1</v>
       </c>
       <c r="D14">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>55</v>
+        <v>28</v>
       </c>
       <c r="B15" t="s">
-        <v>56</v>
+        <v>29</v>
       </c>
       <c r="C15">
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="D15">
-        <v>48</v>
+        <v>6</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>141</v>
+        <v>30</v>
       </c>
       <c r="B16" t="s">
-        <v>142</v>
+        <v>31</v>
       </c>
       <c r="C16">
-        <v>34</v>
+        <v>1</v>
       </c>
       <c r="D16">
         <v>0</v>
@@ -1401,55 +1401,55 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>250</v>
+        <v>32</v>
       </c>
       <c r="B17" t="s">
-        <v>251</v>
+        <v>33</v>
       </c>
       <c r="C17">
-        <v>29</v>
+        <v>4</v>
       </c>
       <c r="D17">
-        <v>53</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>143</v>
+        <v>34</v>
       </c>
       <c r="B18" t="s">
-        <v>144</v>
+        <v>35</v>
       </c>
       <c r="C18">
-        <v>28</v>
+        <v>3</v>
       </c>
       <c r="D18">
-        <v>207</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>238</v>
+        <v>36</v>
       </c>
       <c r="B19" t="s">
-        <v>239</v>
+        <v>37</v>
       </c>
       <c r="C19">
-        <v>27</v>
+        <v>1</v>
       </c>
       <c r="D19">
-        <v>509</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>119</v>
+        <v>38</v>
       </c>
       <c r="B20" t="s">
-        <v>120</v>
+        <v>39</v>
       </c>
       <c r="C20">
-        <v>26</v>
+        <v>3</v>
       </c>
       <c r="D20">
         <v>0</v>
@@ -1457,276 +1457,276 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>155</v>
+        <v>40</v>
       </c>
       <c r="B21" t="s">
-        <v>156</v>
+        <v>41</v>
       </c>
       <c r="C21">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="D21">
-        <v>2</v>
+        <v>232</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" t="s">
-        <v>248</v>
+        <v>42</v>
       </c>
       <c r="B22" t="s">
-        <v>249</v>
+        <v>43</v>
       </c>
       <c r="C22">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="D22">
-        <v>8</v>
+        <v>202</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>145</v>
+        <v>44</v>
       </c>
       <c r="B23" t="s">
-        <v>146</v>
+        <v>45</v>
       </c>
       <c r="C23">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="D23">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>77</v>
+        <v>46</v>
       </c>
       <c r="B24" t="s">
-        <v>78</v>
+        <v>47</v>
       </c>
       <c r="C24">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="D24">
-        <v>0</v>
+        <v>551</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>3</v>
+        <v>48</v>
       </c>
       <c r="B25" t="s">
-        <v>4</v>
+        <v>49</v>
       </c>
       <c r="C25">
-        <v>18</v>
+        <v>94</v>
       </c>
       <c r="D25">
-        <v>0</v>
+        <v>3353</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" t="s">
-        <v>17</v>
+        <v>50</v>
       </c>
       <c r="B26" t="s">
-        <v>18</v>
+        <v>51</v>
       </c>
       <c r="C26">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="D26">
-        <v>0</v>
+        <v>565</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" t="s">
-        <v>244</v>
+        <v>52</v>
       </c>
       <c r="B27" t="s">
-        <v>245</v>
+        <v>53</v>
       </c>
       <c r="C27">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="D27">
-        <v>0</v>
+        <v>2159</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" t="s">
-        <v>89</v>
+        <v>54</v>
       </c>
       <c r="B28" t="s">
-        <v>90</v>
+        <v>55</v>
       </c>
       <c r="C28">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="D28">
-        <v>1</v>
+        <v>48</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" t="s">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="B29" t="s">
-        <v>44</v>
+        <v>57</v>
       </c>
       <c r="C29">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="D29">
-        <v>202</v>
+        <v>165</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" t="s">
-        <v>15</v>
+        <v>58</v>
       </c>
       <c r="B30" t="s">
-        <v>16</v>
+        <v>59</v>
       </c>
       <c r="C30">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="D30">
-        <v>79</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" t="s">
-        <v>41</v>
+        <v>60</v>
       </c>
       <c r="B31" t="s">
-        <v>42</v>
+        <v>61</v>
       </c>
       <c r="C31">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D31">
-        <v>232</v>
+        <v>236</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B32" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C32">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="D32">
-        <v>236</v>
+        <v>1482</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" t="s">
-        <v>173</v>
+        <v>64</v>
       </c>
       <c r="B33" t="s">
-        <v>174</v>
+        <v>65</v>
       </c>
       <c r="C33">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D33">
-        <v>92</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" t="s">
-        <v>183</v>
+        <v>66</v>
       </c>
       <c r="B34" t="s">
-        <v>184</v>
+        <v>67</v>
       </c>
       <c r="C34">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="D34">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" t="s">
-        <v>147</v>
+        <v>68</v>
       </c>
       <c r="B35" t="s">
-        <v>148</v>
+        <v>69</v>
       </c>
       <c r="C35">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="D35">
-        <v>1</v>
+        <v>721</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" t="s">
-        <v>242</v>
+        <v>70</v>
       </c>
       <c r="B36" t="s">
-        <v>243</v>
+        <v>71</v>
       </c>
       <c r="C36">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="D36">
-        <v>199</v>
+        <v>44</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="B37" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="C37">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D37">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" t="s">
-        <v>115</v>
+        <v>74</v>
       </c>
       <c r="B38" t="s">
-        <v>116</v>
+        <v>75</v>
       </c>
       <c r="C38">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="D38">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" t="s">
-        <v>201</v>
+        <v>76</v>
       </c>
       <c r="B39" t="s">
-        <v>202</v>
+        <v>77</v>
       </c>
       <c r="C39">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="D39">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" t="s">
+        <v>78</v>
+      </c>
+      <c r="B40" t="s">
         <v>79</v>
-      </c>
-      <c r="B40" t="s">
-        <v>80</v>
       </c>
       <c r="C40">
         <v>9</v>
@@ -1737,69 +1737,69 @@
     </row>
     <row r="41" spans="1:4">
       <c r="A41" t="s">
-        <v>129</v>
+        <v>80</v>
       </c>
       <c r="B41" t="s">
-        <v>130</v>
+        <v>81</v>
       </c>
       <c r="C41">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D41">
-        <v>430</v>
+        <v>4</v>
       </c>
     </row>
     <row r="42" spans="1:4">
       <c r="A42" t="s">
-        <v>137</v>
+        <v>82</v>
       </c>
       <c r="B42" t="s">
-        <v>138</v>
+        <v>83</v>
       </c>
       <c r="C42">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="D42">
-        <v>86</v>
+        <v>4</v>
       </c>
     </row>
     <row r="43" spans="1:4">
       <c r="A43" t="s">
-        <v>246</v>
+        <v>84</v>
       </c>
       <c r="B43" t="s">
-        <v>247</v>
+        <v>85</v>
       </c>
       <c r="C43">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D43">
-        <v>692</v>
+        <v>2</v>
       </c>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" t="s">
-        <v>53</v>
+        <v>86</v>
       </c>
       <c r="B44" t="s">
-        <v>54</v>
+        <v>87</v>
       </c>
       <c r="C44">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="D44">
-        <v>2159</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:4">
       <c r="A45" t="s">
-        <v>65</v>
+        <v>88</v>
       </c>
       <c r="B45" t="s">
-        <v>66</v>
+        <v>89</v>
       </c>
       <c r="C45">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="D45">
         <v>1</v>
@@ -1807,111 +1807,111 @@
     </row>
     <row r="46" spans="1:4">
       <c r="A46" t="s">
-        <v>125</v>
+        <v>90</v>
       </c>
       <c r="B46" t="s">
-        <v>126</v>
+        <v>91</v>
       </c>
       <c r="C46">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="D46">
-        <v>414</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:4">
       <c r="A47" t="s">
-        <v>165</v>
+        <v>92</v>
       </c>
       <c r="B47" t="s">
-        <v>166</v>
+        <v>93</v>
       </c>
       <c r="C47">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="D47">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:4">
       <c r="A48" t="s">
-        <v>235</v>
+        <v>94</v>
       </c>
       <c r="B48" t="s">
-        <v>234</v>
+        <v>95</v>
       </c>
       <c r="C48">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D48">
-        <v>28845</v>
+        <v>9</v>
       </c>
     </row>
     <row r="49" spans="1:4">
       <c r="A49" t="s">
-        <v>7</v>
+        <v>96</v>
       </c>
       <c r="B49" t="s">
-        <v>8</v>
+        <v>97</v>
       </c>
       <c r="C49">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D49">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:4">
       <c r="A50" t="s">
-        <v>151</v>
+        <v>98</v>
       </c>
       <c r="B50" t="s">
-        <v>152</v>
+        <v>99</v>
       </c>
       <c r="C50">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D50">
-        <v>0</v>
+        <v>11</v>
       </c>
     </row>
     <row r="51" spans="1:4">
       <c r="A51" t="s">
-        <v>187</v>
+        <v>100</v>
       </c>
       <c r="B51" t="s">
-        <v>188</v>
+        <v>101</v>
       </c>
       <c r="C51">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D51">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:4">
       <c r="A52" t="s">
-        <v>205</v>
+        <v>102</v>
       </c>
       <c r="B52" t="s">
-        <v>206</v>
+        <v>103</v>
       </c>
       <c r="C52">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D52">
-        <v>48</v>
+        <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:4">
       <c r="A53" t="s">
-        <v>215</v>
+        <v>104</v>
       </c>
       <c r="B53" t="s">
-        <v>216</v>
+        <v>105</v>
       </c>
       <c r="C53">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D53">
         <v>0</v>
@@ -1919,41 +1919,41 @@
     </row>
     <row r="54" spans="1:4">
       <c r="A54" t="s">
-        <v>9</v>
+        <v>106</v>
       </c>
       <c r="B54" t="s">
-        <v>10</v>
+        <v>107</v>
       </c>
       <c r="C54">
-        <v>6</v>
+        <v>60</v>
       </c>
       <c r="D54">
-        <v>2262</v>
+        <v>430</v>
       </c>
     </row>
     <row r="55" spans="1:4">
       <c r="A55" t="s">
-        <v>57</v>
+        <v>108</v>
       </c>
       <c r="B55" t="s">
-        <v>58</v>
+        <v>109</v>
       </c>
       <c r="C55">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D55">
-        <v>165</v>
+        <v>1</v>
       </c>
     </row>
     <row r="56" spans="1:4">
       <c r="A56" t="s">
-        <v>197</v>
+        <v>110</v>
       </c>
       <c r="B56" t="s">
-        <v>198</v>
+        <v>111</v>
       </c>
       <c r="C56">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D56">
         <v>0</v>
@@ -1961,111 +1961,111 @@
     </row>
     <row r="57" spans="1:4">
       <c r="A57" t="s">
-        <v>233</v>
+        <v>112</v>
       </c>
       <c r="B57" t="s">
-        <v>234</v>
+        <v>113</v>
       </c>
       <c r="C57">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D57">
-        <v>2859</v>
+        <v>1</v>
       </c>
     </row>
     <row r="58" spans="1:4">
       <c r="A58" t="s">
-        <v>236</v>
+        <v>114</v>
       </c>
       <c r="B58" t="s">
-        <v>237</v>
+        <v>115</v>
       </c>
       <c r="C58">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D58">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="59" spans="1:4">
       <c r="A59" t="s">
-        <v>5</v>
+        <v>116</v>
       </c>
       <c r="B59" t="s">
-        <v>6</v>
+        <v>117</v>
       </c>
       <c r="C59">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D59">
-        <v>2</v>
+        <v>225</v>
       </c>
     </row>
     <row r="60" spans="1:4">
       <c r="A60" t="s">
-        <v>85</v>
+        <v>118</v>
       </c>
       <c r="B60" t="s">
-        <v>86</v>
+        <v>119</v>
       </c>
       <c r="C60">
-        <v>5</v>
+        <v>26</v>
       </c>
       <c r="D60">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="61" spans="1:4">
       <c r="A61" t="s">
-        <v>211</v>
+        <v>120</v>
       </c>
       <c r="B61" t="s">
-        <v>212</v>
+        <v>121</v>
       </c>
       <c r="C61">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D61">
-        <v>236</v>
+        <v>0</v>
       </c>
     </row>
     <row r="62" spans="1:4">
       <c r="A62" t="s">
-        <v>217</v>
+        <v>122</v>
       </c>
       <c r="B62" t="s">
-        <v>218</v>
+        <v>123</v>
       </c>
       <c r="C62">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D62">
-        <v>0</v>
+        <v>19</v>
       </c>
     </row>
     <row r="63" spans="1:4">
       <c r="A63" t="s">
-        <v>23</v>
+        <v>124</v>
       </c>
       <c r="B63" t="s">
-        <v>24</v>
+        <v>125</v>
       </c>
       <c r="C63">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D63">
-        <v>44</v>
+        <v>414</v>
       </c>
     </row>
     <row r="64" spans="1:4">
       <c r="A64" t="s">
-        <v>33</v>
+        <v>126</v>
       </c>
       <c r="B64" t="s">
-        <v>34</v>
+        <v>127</v>
       </c>
       <c r="C64">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D64">
         <v>0</v>
@@ -2073,41 +2073,41 @@
     </row>
     <row r="65" spans="1:4">
       <c r="A65" t="s">
-        <v>69</v>
+        <v>128</v>
       </c>
       <c r="B65" t="s">
-        <v>70</v>
+        <v>129</v>
       </c>
       <c r="C65">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D65">
-        <v>721</v>
+        <v>430</v>
       </c>
     </row>
     <row r="66" spans="1:4">
       <c r="A66" t="s">
-        <v>71</v>
+        <v>130</v>
       </c>
       <c r="B66" t="s">
-        <v>72</v>
+        <v>131</v>
       </c>
       <c r="C66">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D66">
-        <v>44</v>
+        <v>0</v>
       </c>
     </row>
     <row r="67" spans="1:4">
       <c r="A67" t="s">
-        <v>21</v>
+        <v>132</v>
       </c>
       <c r="B67" t="s">
-        <v>22</v>
+        <v>133</v>
       </c>
       <c r="C67">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D67">
         <v>0</v>
@@ -2115,13 +2115,13 @@
     </row>
     <row r="68" spans="1:4">
       <c r="A68" t="s">
-        <v>25</v>
+        <v>134</v>
       </c>
       <c r="B68" t="s">
-        <v>26</v>
+        <v>135</v>
       </c>
       <c r="C68">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D68">
         <v>0</v>
@@ -2129,41 +2129,41 @@
     </row>
     <row r="69" spans="1:4">
       <c r="A69" t="s">
-        <v>35</v>
+        <v>136</v>
       </c>
       <c r="B69" t="s">
-        <v>36</v>
+        <v>137</v>
       </c>
       <c r="C69">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="D69">
-        <v>1</v>
+        <v>86</v>
       </c>
     </row>
     <row r="70" spans="1:4">
       <c r="A70" t="s">
-        <v>39</v>
+        <v>138</v>
       </c>
       <c r="B70" t="s">
-        <v>40</v>
+        <v>139</v>
       </c>
       <c r="C70">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D70">
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="71" spans="1:4">
       <c r="A71" t="s">
-        <v>45</v>
+        <v>140</v>
       </c>
       <c r="B71" t="s">
-        <v>46</v>
+        <v>141</v>
       </c>
       <c r="C71">
-        <v>3</v>
+        <v>34</v>
       </c>
       <c r="D71">
         <v>0</v>
@@ -2171,139 +2171,139 @@
     </row>
     <row r="72" spans="1:4">
       <c r="A72" t="s">
-        <v>67</v>
+        <v>142</v>
       </c>
       <c r="B72" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="C72">
-        <v>3</v>
+        <v>28</v>
       </c>
       <c r="D72">
-        <v>0</v>
+        <v>207</v>
       </c>
     </row>
     <row r="73" spans="1:4">
       <c r="A73" t="s">
-        <v>73</v>
+        <v>144</v>
       </c>
       <c r="B73" t="s">
-        <v>74</v>
+        <v>145</v>
       </c>
       <c r="C73">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="D73">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="74" spans="1:4">
       <c r="A74" t="s">
-        <v>95</v>
+        <v>146</v>
       </c>
       <c r="B74" t="s">
-        <v>96</v>
+        <v>147</v>
       </c>
       <c r="C74">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="D74">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="75" spans="1:4">
       <c r="A75" t="s">
-        <v>99</v>
+        <v>148</v>
       </c>
       <c r="B75" t="s">
-        <v>100</v>
+        <v>149</v>
       </c>
       <c r="C75">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D75">
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="76" spans="1:4">
       <c r="A76" t="s">
-        <v>109</v>
+        <v>150</v>
       </c>
       <c r="B76" t="s">
-        <v>110</v>
+        <v>151</v>
       </c>
       <c r="C76">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D76">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="77" spans="1:4">
       <c r="A77" t="s">
-        <v>117</v>
+        <v>152</v>
       </c>
       <c r="B77" t="s">
-        <v>118</v>
+        <v>153</v>
       </c>
       <c r="C77">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D77">
-        <v>225</v>
+        <v>0</v>
       </c>
     </row>
     <row r="78" spans="1:4">
       <c r="A78" t="s">
-        <v>127</v>
+        <v>154</v>
       </c>
       <c r="B78" t="s">
-        <v>128</v>
+        <v>155</v>
       </c>
       <c r="C78">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="D78">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="79" spans="1:4">
       <c r="A79" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="B79" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C79">
+        <v>39</v>
+      </c>
+      <c r="D79">
         <v>3</v>
-      </c>
-      <c r="D79">
-        <v>1</v>
       </c>
     </row>
     <row r="80" spans="1:4">
       <c r="A80" t="s">
-        <v>179</v>
+        <v>158</v>
       </c>
       <c r="B80" t="s">
-        <v>180</v>
+        <v>159</v>
       </c>
       <c r="C80">
         <v>3</v>
       </c>
       <c r="D80">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="81" spans="1:4">
       <c r="A81" t="s">
-        <v>181</v>
+        <v>160</v>
       </c>
       <c r="B81" t="s">
-        <v>182</v>
+        <v>161</v>
       </c>
       <c r="C81">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D81">
         <v>0</v>
@@ -2311,41 +2311,41 @@
     </row>
     <row r="82" spans="1:4">
       <c r="A82" t="s">
-        <v>193</v>
+        <v>162</v>
       </c>
       <c r="B82" t="s">
-        <v>194</v>
+        <v>163</v>
       </c>
       <c r="C82">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D82">
-        <v>27</v>
+        <v>0</v>
       </c>
     </row>
     <row r="83" spans="1:4">
       <c r="A83" t="s">
-        <v>195</v>
+        <v>164</v>
       </c>
       <c r="B83" t="s">
-        <v>196</v>
+        <v>165</v>
       </c>
       <c r="C83">
+        <v>8</v>
+      </c>
+      <c r="D83">
         <v>3</v>
-      </c>
-      <c r="D83">
-        <v>5</v>
       </c>
     </row>
     <row r="84" spans="1:4">
       <c r="A84" t="s">
-        <v>213</v>
+        <v>166</v>
       </c>
       <c r="B84" t="s">
-        <v>214</v>
+        <v>167</v>
       </c>
       <c r="C84">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D84">
         <v>0</v>
@@ -2353,10 +2353,10 @@
     </row>
     <row r="85" spans="1:4">
       <c r="A85" t="s">
-        <v>11</v>
+        <v>168</v>
       </c>
       <c r="B85" t="s">
-        <v>12</v>
+        <v>169</v>
       </c>
       <c r="C85">
         <v>2</v>
@@ -2367,52 +2367,52 @@
     </row>
     <row r="86" spans="1:4">
       <c r="A86" t="s">
-        <v>19</v>
+        <v>170</v>
       </c>
       <c r="B86" t="s">
-        <v>20</v>
+        <v>171</v>
       </c>
       <c r="C86">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D86">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="87" spans="1:4">
       <c r="A87" t="s">
-        <v>51</v>
+        <v>172</v>
       </c>
       <c r="B87" t="s">
-        <v>52</v>
+        <v>173</v>
       </c>
       <c r="C87">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="D87">
-        <v>565</v>
+        <v>92</v>
       </c>
     </row>
     <row r="88" spans="1:4">
       <c r="A88" t="s">
-        <v>63</v>
+        <v>174</v>
       </c>
       <c r="B88" t="s">
-        <v>64</v>
+        <v>175</v>
       </c>
       <c r="C88">
         <v>2</v>
       </c>
       <c r="D88">
-        <v>1482</v>
+        <v>0</v>
       </c>
     </row>
     <row r="89" spans="1:4">
       <c r="A89" t="s">
-        <v>97</v>
+        <v>176</v>
       </c>
       <c r="B89" t="s">
-        <v>98</v>
+        <v>177</v>
       </c>
       <c r="C89">
         <v>2</v>
@@ -2423,27 +2423,27 @@
     </row>
     <row r="90" spans="1:4">
       <c r="A90" t="s">
-        <v>121</v>
+        <v>178</v>
       </c>
       <c r="B90" t="s">
-        <v>122</v>
+        <v>179</v>
       </c>
       <c r="C90">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D90">
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="91" spans="1:4">
       <c r="A91" t="s">
-        <v>133</v>
+        <v>180</v>
       </c>
       <c r="B91" t="s">
-        <v>134</v>
+        <v>181</v>
       </c>
       <c r="C91">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D91">
         <v>0</v>
@@ -2451,55 +2451,55 @@
     </row>
     <row r="92" spans="1:4">
       <c r="A92" t="s">
-        <v>139</v>
+        <v>182</v>
       </c>
       <c r="B92" t="s">
-        <v>140</v>
+        <v>183</v>
       </c>
       <c r="C92">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="D92">
-        <v>15</v>
+        <v>4</v>
       </c>
     </row>
     <row r="93" spans="1:4">
       <c r="A93" t="s">
-        <v>153</v>
+        <v>184</v>
       </c>
       <c r="B93" t="s">
-        <v>154</v>
+        <v>185</v>
       </c>
       <c r="C93">
+        <v>1</v>
+      </c>
+      <c r="D93">
         <v>2</v>
-      </c>
-      <c r="D93">
-        <v>0</v>
       </c>
     </row>
     <row r="94" spans="1:4">
       <c r="A94" t="s">
-        <v>163</v>
+        <v>186</v>
       </c>
       <c r="B94" t="s">
-        <v>164</v>
+        <v>187</v>
       </c>
       <c r="C94">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D94">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="95" spans="1:4">
       <c r="A95" t="s">
-        <v>167</v>
+        <v>188</v>
       </c>
       <c r="B95" t="s">
-        <v>168</v>
+        <v>189</v>
       </c>
       <c r="C95">
-        <v>2</v>
+        <v>76</v>
       </c>
       <c r="D95">
         <v>0</v>
@@ -2507,13 +2507,13 @@
     </row>
     <row r="96" spans="1:4">
       <c r="A96" t="s">
-        <v>169</v>
+        <v>190</v>
       </c>
       <c r="B96" t="s">
-        <v>170</v>
+        <v>191</v>
       </c>
       <c r="C96">
-        <v>2</v>
+        <v>219</v>
       </c>
       <c r="D96">
         <v>0</v>
@@ -2521,153 +2521,153 @@
     </row>
     <row r="97" spans="1:4">
       <c r="A97" t="s">
-        <v>175</v>
+        <v>192</v>
       </c>
       <c r="B97" t="s">
-        <v>176</v>
+        <v>193</v>
       </c>
       <c r="C97">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D97">
-        <v>0</v>
+        <v>27</v>
       </c>
     </row>
     <row r="98" spans="1:4">
       <c r="A98" t="s">
-        <v>177</v>
+        <v>194</v>
       </c>
       <c r="B98" t="s">
-        <v>178</v>
+        <v>195</v>
       </c>
       <c r="C98">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D98">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="99" spans="1:4">
       <c r="A99" t="s">
-        <v>219</v>
+        <v>196</v>
       </c>
       <c r="B99" t="s">
-        <v>220</v>
+        <v>197</v>
       </c>
       <c r="C99">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D99">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="100" spans="1:4">
       <c r="A100" t="s">
-        <v>13</v>
+        <v>198</v>
       </c>
       <c r="B100" t="s">
-        <v>14</v>
+        <v>199</v>
       </c>
       <c r="C100">
         <v>1</v>
       </c>
       <c r="D100">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="101" spans="1:4">
       <c r="A101" t="s">
-        <v>27</v>
+        <v>200</v>
       </c>
       <c r="B101" t="s">
-        <v>28</v>
+        <v>201</v>
       </c>
       <c r="C101">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="D101">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="102" spans="1:4">
       <c r="A102" t="s">
-        <v>31</v>
+        <v>202</v>
       </c>
       <c r="B102" t="s">
-        <v>32</v>
+        <v>203</v>
       </c>
       <c r="C102">
-        <v>1</v>
+        <v>80</v>
       </c>
       <c r="D102">
-        <v>0</v>
+        <v>90</v>
       </c>
     </row>
     <row r="103" spans="1:4">
       <c r="A103" t="s">
-        <v>37</v>
+        <v>204</v>
       </c>
       <c r="B103" t="s">
-        <v>38</v>
+        <v>205</v>
       </c>
       <c r="C103">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D103">
-        <v>0</v>
+        <v>48</v>
       </c>
     </row>
     <row r="104" spans="1:4">
       <c r="A104" t="s">
-        <v>47</v>
+        <v>206</v>
       </c>
       <c r="B104" t="s">
-        <v>48</v>
+        <v>207</v>
       </c>
       <c r="C104">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D104">
-        <v>551</v>
+        <v>6</v>
       </c>
     </row>
     <row r="105" spans="1:4">
       <c r="A105" t="s">
-        <v>59</v>
+        <v>208</v>
       </c>
       <c r="B105" t="s">
-        <v>60</v>
+        <v>209</v>
       </c>
       <c r="C105">
-        <v>1</v>
+        <v>70</v>
       </c>
       <c r="D105">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="106" spans="1:4">
       <c r="A106" t="s">
-        <v>75</v>
+        <v>210</v>
       </c>
       <c r="B106" t="s">
-        <v>76</v>
+        <v>211</v>
       </c>
       <c r="C106">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D106">
-        <v>0</v>
+        <v>236</v>
       </c>
     </row>
     <row r="107" spans="1:4">
       <c r="A107" t="s">
-        <v>87</v>
+        <v>212</v>
       </c>
       <c r="B107" t="s">
-        <v>88</v>
+        <v>213</v>
       </c>
       <c r="C107">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D107">
         <v>0</v>
@@ -2675,13 +2675,13 @@
     </row>
     <row r="108" spans="1:4">
       <c r="A108" t="s">
-        <v>91</v>
+        <v>214</v>
       </c>
       <c r="B108" t="s">
-        <v>92</v>
+        <v>215</v>
       </c>
       <c r="C108">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D108">
         <v>0</v>
@@ -2689,13 +2689,13 @@
     </row>
     <row r="109" spans="1:4">
       <c r="A109" t="s">
-        <v>93</v>
+        <v>216</v>
       </c>
       <c r="B109" t="s">
-        <v>94</v>
+        <v>217</v>
       </c>
       <c r="C109">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D109">
         <v>0</v>
@@ -2703,139 +2703,139 @@
     </row>
     <row r="110" spans="1:4">
       <c r="A110" t="s">
-        <v>101</v>
+        <v>218</v>
       </c>
       <c r="B110" t="s">
-        <v>102</v>
+        <v>219</v>
       </c>
       <c r="C110">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D110">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="111" spans="1:4">
       <c r="A111" t="s">
-        <v>103</v>
+        <v>220</v>
       </c>
       <c r="B111" t="s">
-        <v>104</v>
+        <v>221</v>
       </c>
       <c r="C111">
-        <v>1</v>
+        <v>69</v>
       </c>
       <c r="D111">
-        <v>0</v>
+        <v>11</v>
       </c>
     </row>
     <row r="112" spans="1:4">
       <c r="A112" t="s">
-        <v>105</v>
+        <v>222</v>
       </c>
       <c r="B112" t="s">
-        <v>106</v>
+        <v>223</v>
       </c>
       <c r="C112">
-        <v>1</v>
+        <v>298</v>
       </c>
       <c r="D112">
-        <v>0</v>
+        <v>195</v>
       </c>
     </row>
     <row r="113" spans="1:4">
       <c r="A113" t="s">
-        <v>111</v>
+        <v>224</v>
       </c>
       <c r="B113" t="s">
-        <v>112</v>
+        <v>225</v>
       </c>
       <c r="C113">
-        <v>1</v>
+        <v>106</v>
       </c>
       <c r="D113">
-        <v>0</v>
+        <v>48</v>
       </c>
     </row>
     <row r="114" spans="1:4">
       <c r="A114" t="s">
-        <v>113</v>
+        <v>226</v>
       </c>
       <c r="B114" t="s">
-        <v>114</v>
+        <v>227</v>
       </c>
       <c r="C114">
-        <v>1</v>
+        <v>37</v>
       </c>
       <c r="D114">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="115" spans="1:4">
       <c r="A115" t="s">
-        <v>131</v>
+        <v>228</v>
       </c>
       <c r="B115" t="s">
-        <v>132</v>
+        <v>229</v>
       </c>
       <c r="C115">
-        <v>1</v>
+        <v>51</v>
       </c>
       <c r="D115">
-        <v>0</v>
+        <v>64</v>
       </c>
     </row>
     <row r="116" spans="1:4">
       <c r="A116" t="s">
-        <v>135</v>
+        <v>230</v>
       </c>
       <c r="B116" t="s">
-        <v>136</v>
+        <v>231</v>
       </c>
       <c r="C116">
-        <v>1</v>
+        <v>158</v>
       </c>
       <c r="D116">
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="117" spans="1:4">
       <c r="A117" t="s">
-        <v>161</v>
+        <v>232</v>
       </c>
       <c r="B117" t="s">
-        <v>162</v>
+        <v>233</v>
       </c>
       <c r="C117">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D117">
-        <v>0</v>
+        <v>2859</v>
       </c>
     </row>
     <row r="118" spans="1:4">
       <c r="A118" t="s">
-        <v>171</v>
+        <v>234</v>
       </c>
       <c r="B118" t="s">
-        <v>172</v>
+        <v>233</v>
       </c>
       <c r="C118">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D118">
-        <v>0</v>
+        <v>28845</v>
       </c>
     </row>
     <row r="119" spans="1:4">
       <c r="A119" t="s">
-        <v>185</v>
+        <v>235</v>
       </c>
       <c r="B119" t="s">
-        <v>186</v>
+        <v>236</v>
       </c>
       <c r="C119">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D119">
         <v>2</v>
@@ -2843,24 +2843,24 @@
     </row>
     <row r="120" spans="1:4">
       <c r="A120" t="s">
-        <v>199</v>
+        <v>237</v>
       </c>
       <c r="B120" t="s">
-        <v>200</v>
+        <v>238</v>
       </c>
       <c r="C120">
-        <v>1</v>
+        <v>27</v>
       </c>
       <c r="D120">
-        <v>0</v>
+        <v>509</v>
       </c>
     </row>
     <row r="121" spans="1:4">
       <c r="A121" t="s">
+        <v>239</v>
+      </c>
+      <c r="B121" t="s">
         <v>240</v>
-      </c>
-      <c r="B121" t="s">
-        <v>241</v>
       </c>
       <c r="C121">
         <v>1</v>
@@ -2871,72 +2871,72 @@
     </row>
     <row r="122" spans="1:4">
       <c r="A122" t="s">
-        <v>29</v>
+        <v>241</v>
       </c>
       <c r="B122" t="s">
-        <v>30</v>
+        <v>242</v>
       </c>
       <c r="C122">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="D122">
-        <v>6</v>
+        <v>199</v>
       </c>
     </row>
     <row r="123" spans="1:4">
       <c r="A123" t="s">
-        <v>83</v>
+        <v>243</v>
       </c>
       <c r="B123" t="s">
-        <v>84</v>
+        <v>244</v>
       </c>
       <c r="C123">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="D123">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="124" spans="1:4">
       <c r="A124" t="s">
-        <v>123</v>
+        <v>245</v>
       </c>
       <c r="B124" t="s">
-        <v>124</v>
+        <v>246</v>
       </c>
       <c r="C124">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="D124">
-        <v>19</v>
+        <v>692</v>
       </c>
     </row>
     <row r="125" spans="1:4">
       <c r="A125" t="s">
-        <v>149</v>
+        <v>247</v>
       </c>
       <c r="B125" t="s">
-        <v>150</v>
+        <v>248</v>
       </c>
       <c r="C125">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="D125">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="126" spans="1:4">
       <c r="A126" t="s">
-        <v>207</v>
+        <v>249</v>
       </c>
       <c r="B126" t="s">
-        <v>208</v>
+        <v>250</v>
       </c>
       <c r="C126">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="D126">
-        <v>6</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>